<commit_message>
2023-04-27 save compressed csv files is now defined by a parameter
</commit_message>
<xml_diff>
--- a/EU_random_points.xlsx
+++ b/EU_random_points.xlsx
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,12 +109,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,1154 +160,1154 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>58.053</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>-6.577</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>41.476</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>-5.85</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>37.832</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>-5.29</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>39.675</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>-5.028</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>43.133</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>-4.265</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>57.09</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>-3.293</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>51.897</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>-3.214</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>38.783</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>-2.744</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>38.441</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>-2.577</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>50.958</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>-1.462</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>59.942</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>-1.272</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>46.303</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>-0.573</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>44.249</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>0.23</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>40.79</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>0.51</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>43.248</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>0.658</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>51.916</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>4.148</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>46.692</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>4.412</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>44.161</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>4.936</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>51.536</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>6.356</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>60.287</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>6.948</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>46.266</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>7.223</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>61.312</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>8.351</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>44.547</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>8.869</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>59.144</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>9.034</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>49.687</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>9.501</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>59.948</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>9.955</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>61.209</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>10.505</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>46.423</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>10.58</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>54.269</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>10.734</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>46.958</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>11.581</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>43.909</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="1" t="n">
         <v>11.693</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="1" t="n">
         <v>47.47</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="1" t="n">
         <v>11.801</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>45.955</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <v>11.837</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <v>41.74</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="1" t="n">
         <v>12.322</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <v>57.41</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <v>13.624</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>59.063</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="1" t="n">
         <v>14.021</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <v>57.005</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38" s="1" t="n">
         <v>14.403</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <v>52.546</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <v>14.807</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="1" t="n">
         <v>37.903</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40" s="1" t="n">
         <v>15.046</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="1" t="n">
         <v>61.049</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="1" t="n">
         <v>15.575</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <v>48.922</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="1" t="n">
         <v>16.92</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <v>50.842</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="1" t="n">
         <v>17.014</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <v>46.986</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44" s="1" t="n">
         <v>17.361</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>54.196</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="C45" s="1" t="n">
         <v>17.86</v>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="D45" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <v>47.717</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46" s="1" t="n">
         <v>18.415</v>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="D46" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="1" t="n">
         <v>49.934</v>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="C47" s="1" t="n">
         <v>19.907</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="1" t="n">
         <v>52.15</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="1" t="n">
         <v>19.908</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B49" s="1" t="n">
         <v>54.833</v>
       </c>
-      <c r="C49" s="0" t="n">
+      <c r="C49" s="1" t="n">
         <v>20.329</v>
       </c>
-      <c r="D49" s="0" t="n">
+      <c r="D49" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+      <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="1" t="n">
         <v>51.81</v>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="C50" s="1" t="n">
         <v>20.51</v>
       </c>
-      <c r="D50" s="0" t="n">
+      <c r="D50" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="1" t="n">
         <v>40.261</v>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="C51" s="1" t="n">
         <v>20.8</v>
       </c>
-      <c r="D51" s="0" t="n">
+      <c r="D51" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="0" t="n">
+      <c r="B52" s="1" t="n">
         <v>39.182</v>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="C52" s="1" t="n">
         <v>21.787</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="D52" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="0" t="n">
+      <c r="B53" s="1" t="n">
         <v>44.802</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53" s="1" t="n">
         <v>22.26</v>
       </c>
-      <c r="D53" s="0" t="n">
+      <c r="D53" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="A54" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="0" t="n">
+      <c r="B54" s="1" t="n">
         <v>38.686</v>
       </c>
-      <c r="C54" s="0" t="n">
+      <c r="C54" s="1" t="n">
         <v>22.337</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="0" t="n">
+      <c r="B55" s="1" t="n">
         <v>38.606</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55" s="1" t="n">
         <v>22.359</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
+      <c r="A56" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="0" t="n">
+      <c r="B56" s="1" t="n">
         <v>49.817</v>
       </c>
-      <c r="C56" s="0" t="n">
+      <c r="C56" s="1" t="n">
         <v>22.381</v>
       </c>
-      <c r="D56" s="0" t="n">
+      <c r="D56" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="0" t="n">
+      <c r="B57" s="1" t="n">
         <v>55.671</v>
       </c>
-      <c r="C57" s="0" t="n">
+      <c r="C57" s="1" t="n">
         <v>22.621</v>
       </c>
-      <c r="D57" s="0" t="n">
+      <c r="D57" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
+      <c r="A58" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="1" t="n">
         <v>53.768</v>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="C58" s="1" t="n">
         <v>24.026</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="1" t="n">
         <v>57.756</v>
       </c>
-      <c r="C59" s="0" t="n">
+      <c r="C59" s="1" t="n">
         <v>24.976</v>
       </c>
-      <c r="D59" s="0" t="n">
+      <c r="D59" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
+      <c r="A60" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="1" t="n">
         <v>57.001</v>
       </c>
-      <c r="C60" s="0" t="n">
+      <c r="C60" s="1" t="n">
         <v>25.043</v>
       </c>
-      <c r="D60" s="0" t="n">
+      <c r="D60" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="0" t="n">
+      <c r="B61" s="1" t="n">
         <v>57.616</v>
       </c>
-      <c r="C61" s="0" t="n">
+      <c r="C61" s="1" t="n">
         <v>25.281</v>
       </c>
-      <c r="D61" s="0" t="n">
+      <c r="D61" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+      <c r="A62" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="0" t="n">
+      <c r="B62" s="1" t="n">
         <v>49.849</v>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="C62" s="1" t="n">
         <v>25.651</v>
       </c>
-      <c r="D62" s="0" t="n">
+      <c r="D62" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="1" t="n">
         <v>55.689</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C63" s="1" t="n">
         <v>25.749</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D63" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="A64" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="0" t="n">
+      <c r="B64" s="1" t="n">
         <v>58.073</v>
       </c>
-      <c r="C64" s="0" t="n">
+      <c r="C64" s="1" t="n">
         <v>25.781</v>
       </c>
-      <c r="D64" s="0" t="n">
+      <c r="D64" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="0" t="n">
+      <c r="B65" s="1" t="n">
         <v>52.982</v>
       </c>
-      <c r="C65" s="0" t="n">
+      <c r="C65" s="1" t="n">
         <v>26.007</v>
       </c>
-      <c r="D65" s="0" t="n">
+      <c r="D65" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
+      <c r="A66" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="0" t="n">
+      <c r="B66" s="1" t="n">
         <v>47.366</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C66" s="1" t="n">
         <v>26.587</v>
       </c>
-      <c r="D66" s="0" t="n">
+      <c r="D66" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
+      <c r="A67" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="1" t="n">
         <v>37.695</v>
       </c>
-      <c r="C67" s="0" t="n">
+      <c r="C67" s="1" t="n">
         <v>26.606</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D67" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
+      <c r="A68" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="0" t="n">
+      <c r="B68" s="1" t="n">
         <v>49.902</v>
       </c>
-      <c r="C68" s="0" t="n">
+      <c r="C68" s="1" t="n">
         <v>26.606</v>
       </c>
-      <c r="D68" s="0" t="n">
+      <c r="D68" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
+      <c r="A69" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="0" t="n">
+      <c r="B69" s="1" t="n">
         <v>61.44</v>
       </c>
-      <c r="C69" s="0" t="n">
+      <c r="C69" s="1" t="n">
         <v>27.063</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D69" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
+      <c r="A70" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="1" t="n">
         <v>52.58</v>
       </c>
-      <c r="C70" s="0" t="n">
+      <c r="C70" s="1" t="n">
         <v>27.095</v>
       </c>
-      <c r="D70" s="0" t="n">
+      <c r="D70" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
+      <c r="A71" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="0" t="n">
+      <c r="B71" s="1" t="n">
         <v>54.708</v>
       </c>
-      <c r="C71" s="0" t="n">
+      <c r="C71" s="1" t="n">
         <v>27.117</v>
       </c>
-      <c r="D71" s="0" t="n">
+      <c r="D71" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
+      <c r="A72" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="0" t="n">
+      <c r="B72" s="1" t="n">
         <v>45.824</v>
       </c>
-      <c r="C72" s="0" t="n">
+      <c r="C72" s="1" t="n">
         <v>28.107</v>
       </c>
-      <c r="D72" s="0" t="n">
+      <c r="D72" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
+      <c r="A73" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="0" t="n">
+      <c r="B73" s="1" t="n">
         <v>56.727</v>
       </c>
-      <c r="C73" s="0" t="n">
+      <c r="C73" s="1" t="n">
         <v>28.415</v>
       </c>
-      <c r="D73" s="0" t="n">
+      <c r="D73" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
+      <c r="A74" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="0" t="n">
+      <c r="B74" s="1" t="n">
         <v>53.874</v>
       </c>
-      <c r="C74" s="0" t="n">
+      <c r="C74" s="1" t="n">
         <v>29.075</v>
       </c>
-      <c r="D74" s="0" t="n">
+      <c r="D74" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
+      <c r="A75" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="0" t="n">
+      <c r="B75" s="1" t="n">
         <v>49.547</v>
       </c>
-      <c r="C75" s="0" t="n">
+      <c r="C75" s="1" t="n">
         <v>30.276</v>
       </c>
-      <c r="D75" s="0" t="n">
+      <c r="D75" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="n">
+      <c r="A76" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="0" t="n">
+      <c r="B76" s="1" t="n">
         <v>53.57</v>
       </c>
-      <c r="C76" s="0" t="n">
+      <c r="C76" s="1" t="n">
         <v>32.624</v>
       </c>
-      <c r="D76" s="0" t="n">
+      <c r="D76" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
+      <c r="A77" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="0" t="n">
+      <c r="B77" s="1" t="n">
         <v>47.829</v>
       </c>
-      <c r="C77" s="0" t="n">
+      <c r="C77" s="1" t="n">
         <v>33.99</v>
       </c>
-      <c r="D77" s="0" t="n">
+      <c r="D77" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="n">
+      <c r="A78" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="0" t="n">
+      <c r="B78" s="1" t="n">
         <v>48.06</v>
       </c>
-      <c r="C78" s="0" t="n">
+      <c r="C78" s="1" t="n">
         <v>34.547</v>
       </c>
-      <c r="D78" s="0" t="n">
+      <c r="D78" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
+      <c r="A79" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="0" t="n">
+      <c r="B79" s="1" t="n">
         <v>45.218</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="1" t="n">
         <v>35.487</v>
       </c>
-      <c r="D79" s="0" t="n">
+      <c r="D79" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="n">
+      <c r="A80" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="0" t="n">
+      <c r="B80" s="1" t="n">
         <v>50.213</v>
       </c>
-      <c r="C80" s="0" t="n">
+      <c r="C80" s="1" t="n">
         <v>35.661</v>
       </c>
-      <c r="D80" s="0" t="n">
+      <c r="D80" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
+      <c r="A81" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="0" t="n">
+      <c r="B81" s="1" t="n">
         <v>48.649</v>
       </c>
-      <c r="C81" s="0" t="n">
+      <c r="C81" s="1" t="n">
         <v>38.744</v>
       </c>
-      <c r="D81" s="0" t="n">
+      <c r="D81" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
+      <c r="A82" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="0" t="n">
+      <c r="B82" s="1" t="n">
         <v>48.548</v>
       </c>
-      <c r="C82" s="0" t="n">
+      <c r="C82" s="1" t="n">
         <v>39.668</v>
       </c>
-      <c r="D82" s="0" t="n">
+      <c r="D82" s="1" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>